<commit_message>
Webpage For Leetcode top 75 questions NeetCode YT blind75
</commit_message>
<xml_diff>
--- a/Leetcode 75 Questions.xlsx
+++ b/Leetcode 75 Questions.xlsx
@@ -13,7 +13,24 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="316">
   <si>
-    <t>Video Solution</t>
+    <r>
+      <rPr>
+        <rFont val="EB Garamond"/>
+        <b/>
+        <color theme="1"/>
+        <sz val="10.0"/>
+      </rPr>
+      <t xml:space="preserve">Video </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="EB Garamond"/>
+        <b/>
+        <color theme="1"/>
+        <sz val="11.0"/>
+      </rPr>
+      <t>Solution</t>
+    </r>
   </si>
   <si>
     <t>Category</t>
@@ -965,11 +982,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="14">
+  <fonts count="15">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10.0"/>
+      <color theme="1"/>
+      <name val="EB Garamond"/>
     </font>
     <font>
       <b/>
@@ -1140,49 +1163,49 @@
     <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="2" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="2" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="2" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="2" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="2" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="2" fillId="5" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="2" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="2" fillId="6" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="2" fillId="5" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="1" fillId="7" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="2" fillId="6" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="2" fillId="8" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="1" fillId="7" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="1" fillId="9" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="2" fillId="8" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="2" fillId="10" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="1" fillId="9" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="2" fillId="10" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="13" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="14" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -1400,7 +1423,7 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="14.71"/>
-    <col customWidth="1" min="2" max="2" width="26.43"/>
+    <col customWidth="1" min="2" max="2" width="23.86"/>
     <col customWidth="1" min="3" max="3" width="40.43"/>
     <col customWidth="1" min="4" max="4" width="19.43"/>
     <col customWidth="1" min="5" max="5" width="167.57"/>
@@ -1427,23 +1450,6 @@
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="3"/>
-      <c r="S1" s="3"/>
-      <c r="T1" s="3"/>
-      <c r="U1" s="3"/>
-      <c r="V1" s="3"/>
-      <c r="W1" s="3"/>
-      <c r="X1" s="3"/>
-      <c r="Y1" s="3"/>
-      <c r="Z1" s="3"/>
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="4" t="s">

</xml_diff>